<commit_message>
prepare test cases and function library
</commit_message>
<xml_diff>
--- a/TestInput/HybridData.xlsx
+++ b/TestInput/HybridData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>TCID</t>
   </si>
@@ -79,13 +79,112 @@
   </si>
   <si>
     <t>TestData</t>
+  </si>
+  <si>
+    <t>Launch browser</t>
+  </si>
+  <si>
+    <t>startBrowser</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Launch url in a browser</t>
+  </si>
+  <si>
+    <t>openApplication</t>
+  </si>
+  <si>
+    <t>wait for username</t>
+  </si>
+  <si>
+    <t>waitForElement</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>typeAction</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>wait for password</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>wait for login button</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>click login</t>
+  </si>
+  <si>
+    <t>clickAction</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>btnsubmit</t>
+  </si>
+  <si>
+    <t>wait for logout</t>
+  </si>
+  <si>
+    <t>//a[@id='logout']</t>
+  </si>
+  <si>
+    <t>verify title</t>
+  </si>
+  <si>
+    <t>validateTitle</t>
+  </si>
+  <si>
+    <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>click logout</t>
+  </si>
+  <si>
+    <t>wait for ok button</t>
+  </si>
+  <si>
+    <t>click ok button</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +199,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -128,9 +233,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +620,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="5" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75">
@@ -549,8 +654,264 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
wrote test cases for supplier module
</commit_message>
<xml_diff>
--- a/TestInput/HybridData.xlsx
+++ b/TestInput/HybridData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
     <sheet name="ApplicationLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Suppliers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="94">
   <si>
     <t>TCID</t>
   </si>
@@ -69,18 +69,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>FunctionName</t>
-  </si>
-  <si>
-    <t>LocatorType</t>
-  </si>
-  <si>
-    <t>LocatorValue</t>
-  </si>
-  <si>
-    <t>TestData</t>
-  </si>
-  <si>
     <t>Launch browser</t>
   </si>
   <si>
@@ -178,13 +166,145 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>wait for supplier link</t>
+  </si>
+  <si>
+    <t>//body/div[2]/div[2]/div[1]/div[1]/ul[1]/li[3]/a[1]</t>
+  </si>
+  <si>
+    <t>click on supplier link</t>
+  </si>
+  <si>
+    <t>wait for add + icon button</t>
+  </si>
+  <si>
+    <t>//body/div[2]/div[3]/div[1]/div[1]/div[3]/div[1]/div[1]/div[1]/div[1]/a[1]</t>
+  </si>
+  <si>
+    <t>click on add + icon</t>
+  </si>
+  <si>
+    <t>wait for supplier number</t>
+  </si>
+  <si>
+    <t>capture supplier number</t>
+  </si>
+  <si>
+    <t>captureData</t>
+  </si>
+  <si>
+    <t>x_Supplier_Number</t>
+  </si>
+  <si>
+    <t>Enter supplier name</t>
+  </si>
+  <si>
+    <t>Lg suppliers</t>
+  </si>
+  <si>
+    <t>Enter address</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Enter city</t>
+  </si>
+  <si>
+    <t>Kukatpally</t>
+  </si>
+  <si>
+    <t>Enter country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Enter contact person</t>
+  </si>
+  <si>
+    <t>Lg MD</t>
+  </si>
+  <si>
+    <t>Enter phone number</t>
+  </si>
+  <si>
+    <t>25154565555'</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Enter mobile number</t>
+  </si>
+  <si>
+    <t>565456545656'</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Supplier lg goods</t>
+  </si>
+  <si>
+    <t>click add button</t>
+  </si>
+  <si>
+    <t>x_Supplier_Name</t>
+  </si>
+  <si>
+    <t>x_Address</t>
+  </si>
+  <si>
+    <t>x_City</t>
+  </si>
+  <si>
+    <t>x_Country</t>
+  </si>
+  <si>
+    <t>x_Contact_Person</t>
+  </si>
+  <si>
+    <t>x_Phone_Number</t>
+  </si>
+  <si>
+    <t>x__Email</t>
+  </si>
+  <si>
+    <t>x_Mobile_Number</t>
+  </si>
+  <si>
+    <t>x_Notes</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'OK!')]</t>
+  </si>
+  <si>
+    <t>click alert ok button</t>
+  </si>
+  <si>
+    <t>//body/div[17]/div[2]/div[1]/div[4]/div[2]/button[1]</t>
+  </si>
+  <si>
+    <t>validate table</t>
+  </si>
+  <si>
+    <t>suppliertable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +326,28 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -221,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -229,16 +371,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -576,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -622,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,16 +806,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -656,50 +823,50 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -707,33 +874,33 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -741,33 +908,33 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -775,33 +942,33 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -809,33 +976,33 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -843,33 +1010,33 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -877,36 +1044,36 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -917,12 +1084,590 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="66.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E24" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
supplier stock item test cases
</commit_message>
<xml_diff>
--- a/TestInput/HybridData.xlsx
+++ b/TestInput/HybridData.xlsx
@@ -10,13 +10,14 @@
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
     <sheet name="ApplicationLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Suppliers" sheetId="3" r:id="rId3"/>
+    <sheet name="StockItems" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
   <si>
     <t>TCID</t>
   </si>
@@ -298,6 +299,93 @@
   </si>
   <si>
     <t>suppliertable</t>
+  </si>
+  <si>
+    <t>FunctionName</t>
+  </si>
+  <si>
+    <t>LocatorType</t>
+  </si>
+  <si>
+    <t>LocatorValue</t>
+  </si>
+  <si>
+    <t>testData</t>
+  </si>
+  <si>
+    <t>wait for stock items</t>
+  </si>
+  <si>
+    <t>mouseOver</t>
+  </si>
+  <si>
+    <t>Locatortype</t>
+  </si>
+  <si>
+    <t>Locatorvalue</t>
+  </si>
+  <si>
+    <t>Launch Browser</t>
+  </si>
+  <si>
+    <t>Launch url in Browser</t>
+  </si>
+  <si>
+    <t>wait For Username</t>
+  </si>
+  <si>
+    <t>wait for Login button</t>
+  </si>
+  <si>
+    <t>click login button</t>
+  </si>
+  <si>
+    <t>//*[@id='mi_a_stock_items']</t>
+  </si>
+  <si>
+    <t>Mouse Click</t>
+  </si>
+  <si>
+    <t>wait for add button</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t>Click on add icon button</t>
+  </si>
+  <si>
+    <t>wait for Category Name</t>
+  </si>
+  <si>
+    <t>x_Category_Name</t>
+  </si>
+  <si>
+    <t>Enter Category Name</t>
+  </si>
+  <si>
+    <t>Mens</t>
+  </si>
+  <si>
+    <t>click on add button</t>
+  </si>
+  <si>
+    <t>wait for confirm ok button</t>
+  </si>
+  <si>
+    <t>click confirm ok button</t>
+  </si>
+  <si>
+    <t>wait for alert ok button</t>
+  </si>
+  <si>
+    <t>click on alert ok</t>
+  </si>
+  <si>
+    <t>stockTable</t>
+  </si>
+  <si>
+    <t>//button[@id='btnAction']</t>
   </si>
 </sst>
 </file>
@@ -394,7 +482,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -403,6 +491,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -701,7 +792,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -754,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1086,15 +1177,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="66.28515625" customWidth="1"/>
     <col min="5" max="5" width="31.28515625" customWidth="1"/>
   </cols>
@@ -1104,16 +1195,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1276,7 +1367,7 @@
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1290,7 +1381,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1670,4 +1761,460 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="A2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="9">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="9">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="A7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="9">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="A9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75">
+      <c r="A11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="10">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75">
+      <c r="A12" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75">
+      <c r="A13" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="10">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="A14" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="A15" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="10">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="A16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75">
+      <c r="A17" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="10">
+        <v>10</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75">
+      <c r="A18" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75">
+      <c r="A19" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="10">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75">
+      <c r="A21" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="10">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75">
+      <c r="A22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="A23" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75">
+      <c r="A24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>